<commit_message>
Python Code to determine how far platform needs to move
+Tested X axis

*Need to implement other 5 axis
</commit_message>
<xml_diff>
--- a/Joes Stuff/Test/Test_Data1.xlsx
+++ b/Joes Stuff/Test/Test_Data1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\video-to-platform\Joes Stuff\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D25EB9C-E163-4A58-9497-1816C65D3AF9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B55B4B6-AA3A-42B0-8769-9AA3F4938811}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0DC797EE-C7E2-4CD2-BA47-F86046EC79DF}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{0DC797EE-C7E2-4CD2-BA47-F86046EC79DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,6 +95,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B783DEB8-B055-4707-AF41-0E1D758D32AE}" name="Table4" displayName="Table4" ref="A1:F8" totalsRowShown="0">
+  <autoFilter ref="A1:F8" xr:uid="{69503851-804B-4DB5-91C7-E2DC657FADFB}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{0BC7CB5A-79CF-4621-8D79-3843FB7613A9}" name="x"/>
+    <tableColumn id="2" xr3:uid="{408EB04C-F417-4DF5-A7A7-94473996986D}" name="y"/>
+    <tableColumn id="3" xr3:uid="{43A86709-E2B4-4614-8C7B-BD6491FD97DA}" name="z"/>
+    <tableColumn id="4" xr3:uid="{BA86E7C8-4AC1-48CF-88A9-1F5C498DAAB9}" name="x0"/>
+    <tableColumn id="5" xr3:uid="{6A7E5166-7448-417D-80D4-4AAF69DE6CB3}" name="y0"/>
+    <tableColumn id="6" xr3:uid="{CBE1124A-41D6-4363-8CAE-C311F01E17AF}" name="z0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -394,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599C03A3-0F40-4D26-87DD-4523AAA2DAB6}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="I10" sqref="I9:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,67 +457,70 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0.5</v>
-      </c>
-      <c r="B3">
-        <v>0.25</v>
-      </c>
-      <c r="C3">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D3">
-        <v>-0.65</v>
-      </c>
-      <c r="E3">
-        <v>0.76</v>
-      </c>
-      <c r="F3">
-        <v>0.5</v>
-      </c>
-    </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>0.5</v>
+      </c>
+      <c r="B4">
+        <v>0.25</v>
+      </c>
+      <c r="C4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D4">
+        <v>-0.65</v>
+      </c>
+      <c r="E4">
+        <v>0.76</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>0.98</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>0.87</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>0.76</v>
       </c>
-      <c r="E4">
+      <c r="E6">
         <v>0.35</v>
       </c>
-      <c r="F4">
+      <c r="F6">
         <v>0.98</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>0.25</v>
       </c>
-      <c r="B5">
+      <c r="B8">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C8">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="D8">
         <v>0.25</v>
       </c>
-      <c r="E5">
+      <c r="E8">
         <v>0.77</v>
       </c>
-      <c r="F5">
+      <c r="F8">
         <v>0.87</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>